<commit_message>
input all data for A1
</commit_message>
<xml_diff>
--- a/A1/data.xlsx
+++ b/A1/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\inohaan\projects\experiment-3s\A1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED4DBD0-F862-491B-90E7-FBFE3ED04015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFD4913-C2B9-4833-A731-2EF3367709BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="10" xr2:uid="{CC1EBD1F-D9AF-4E74-890C-C2598D192F15}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="9" xr2:uid="{CC1EBD1F-D9AF-4E74-890C-C2598D192F15}"/>
   </bookViews>
   <sheets>
     <sheet name="(1)" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
   <si>
     <t>V_m</t>
     <phoneticPr fontId="1"/>
@@ -104,15 +104,15 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>s</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>f</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Hz</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ms</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -159,8 +159,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -865,45 +868,119 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B948F1C-37CF-438B-A604-B98FD6534051}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1">
+        <v>0.372</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="B4">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="B5">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1">
+        <v>1.21</v>
+      </c>
+      <c r="B6">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1">
+        <v>1.41</v>
+      </c>
+      <c r="B7">
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B8">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1">
+        <v>5.04</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1">
+        <v>6.96</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1">
+        <v>7.96</v>
+      </c>
+      <c r="B12">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1">
+        <v>2.88</v>
+      </c>
+      <c r="B13">
+        <v>7.68</v>
       </c>
     </row>
   </sheetData>
@@ -914,17 +991,21 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DCEB73-F496-4548-A78E-6122D1B7AA10}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -938,7 +1019,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -947,20 +1028,314 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>1.52</v>
       </c>
       <c r="D3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>2.46</v>
+      </c>
+      <c r="C4">
+        <v>2.48</v>
+      </c>
+      <c r="D4">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>2.5</v>
+      </c>
+      <c r="C5">
+        <v>3.92</v>
+      </c>
+      <c r="D5">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>2.5</v>
+      </c>
+      <c r="C6">
+        <v>4.84</v>
+      </c>
+      <c r="D6">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <v>2.4</v>
+      </c>
+      <c r="C7">
+        <v>5.52</v>
+      </c>
+      <c r="D7">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>120</v>
+      </c>
+      <c r="B8">
+        <v>2.46</v>
+      </c>
+      <c r="C8">
+        <v>5.8</v>
+      </c>
+      <c r="D8">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>150</v>
+      </c>
+      <c r="B9">
+        <v>2.4</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>-3.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>200</v>
+      </c>
+      <c r="B10">
+        <v>2.46</v>
+      </c>
+      <c r="C10">
+        <v>6.2</v>
+      </c>
+      <c r="D10">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>250</v>
+      </c>
+      <c r="B11">
+        <v>2.46</v>
+      </c>
+      <c r="C11">
+        <v>6.24</v>
+      </c>
+      <c r="D11">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>300</v>
+      </c>
+      <c r="B12">
+        <v>2.48</v>
+      </c>
+      <c r="C12">
+        <v>6.4</v>
+      </c>
+      <c r="D12">
+        <v>-1.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>400</v>
+      </c>
+      <c r="B13">
+        <v>2.46</v>
+      </c>
+      <c r="C13">
+        <v>6.4</v>
+      </c>
+      <c r="D13">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>500</v>
+      </c>
+      <c r="B14">
+        <v>2.48</v>
+      </c>
+      <c r="C14">
+        <v>6.4</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>700</v>
+      </c>
+      <c r="B15">
+        <v>2.48</v>
+      </c>
+      <c r="C15">
+        <v>6.4</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-0.745</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>1000</v>
+      </c>
+      <c r="B16">
+        <v>2.46</v>
+      </c>
+      <c r="C16">
+        <v>6.4</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>2000</v>
+      </c>
+      <c r="B17">
+        <v>2.44</v>
+      </c>
+      <c r="C17">
+        <v>6.56</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B18">
+        <v>2.48</v>
+      </c>
+      <c r="C18">
+        <v>6.4</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B19">
+        <v>2.42</v>
+      </c>
+      <c r="C19">
+        <v>6.4</v>
+      </c>
+      <c r="D19" s="1">
+        <v>5.28E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1">
+        <v>20000</v>
+      </c>
+      <c r="B20">
+        <v>2.42</v>
+      </c>
+      <c r="C20">
+        <v>5.92</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B21">
+        <v>2.42</v>
+      </c>
+      <c r="C21">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-7.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B22">
+        <v>2.42</v>
+      </c>
+      <c r="C22">
+        <v>2.88</v>
+      </c>
+      <c r="D22" s="1">
+        <v>6.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1">
+        <v>200000</v>
+      </c>
+      <c r="B23">
+        <v>2.42</v>
+      </c>
+      <c r="C23">
+        <v>1.68</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="1">
+        <v>500000</v>
+      </c>
+      <c r="B24">
+        <v>2.4</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D24" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>